<commit_message>
My version of SWE
This is just my version of the SWE.
</commit_message>
<xml_diff>
--- a/SWE/verts.xlsx
+++ b/SWE/verts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\Verts\MTSU Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/727e18b1e1ec388a/Desktop/SWE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA9277E-099A-4835-A945-9D74A2A72D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{BDA9277E-099A-4835-A945-9D74A2A72D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A663DD8F-0198-4C65-AC7D-141C03E0D30E}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vertebrae" sheetId="13" r:id="rId1"/>
@@ -819,6 +819,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DACE3ED4-1BCE-2A75-7A62-51628A62C371}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12199620" y="29809440"/>
+          <a:ext cx="6507480" cy="9753600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1110,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T164" sqref="T164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -14382,5 +14448,6 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>